<commit_message>
Commit document homework 4. Need to do: change history.
</commit_message>
<xml_diff>
--- a/Change_history.xlsx
+++ b/Change_history.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
   <si>
     <t>Revision</t>
   </si>
@@ -180,6 +180,22 @@
   </si>
   <si>
     <t>Modify Measurement.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write the homework 4.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>鍾承翰、楊子冊、吳彥銘</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:40 - 18:50</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -537,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -564,43 +580,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -631,9 +617,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -645,30 +628,68 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -986,113 +1007,113 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="12">
         <v>43168</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+      <c r="B6" s="38">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="42">
         <v>43182</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="43"/>
     </row>
     <row r="8" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="15"/>
+      <c r="D8" s="43"/>
     </row>
     <row r="9" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="15"/>
+      <c r="D9" s="43"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="15"/>
+      <c r="D10" s="43"/>
     </row>
     <row r="11" spans="2:5" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
+      <c r="B12" s="38">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="46">
         <v>43193</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="47"/>
     </row>
     <row r="14" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="45"/>
+      <c r="C14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="47"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="10">
+      <c r="B15" s="38">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="40">
         <v>43203</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="40"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="21"/>
-      <c r="C18" s="22" t="s">
+      <c r="B18" s="39"/>
+      <c r="C18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="23"/>
+      <c r="D18" s="41"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
@@ -1116,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H14"/>
+  <dimension ref="B1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1131,284 +1152,528 @@
     <col min="6" max="6" width="25.42578125" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+    <row r="1" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28">
+      <c r="J2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="19">
         <v>43166</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="33">
+      <c r="F3" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="23">
         <v>60</v>
       </c>
-      <c r="H3" s="34">
+      <c r="H3" s="24">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="35">
+      <c r="J3" s="18">
+        <v>1</v>
+      </c>
+      <c r="K3" s="19">
+        <v>43166</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="21"/>
+      <c r="N3" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="23"/>
+      <c r="P3" s="24"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="49">
         <v>2</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="25">
         <v>43178</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="40">
+      <c r="F4" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="29">
         <v>105</v>
       </c>
-      <c r="H4" s="41">
+      <c r="H4" s="48">
         <f>SUM(G4:G10)</f>
         <v>790</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="35"/>
-      <c r="C5" s="36">
+      <c r="J4" s="18">
+        <v>2</v>
+      </c>
+      <c r="K4" s="25">
         <v>43178</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="L4" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="27"/>
+      <c r="N4" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="29"/>
+      <c r="P4" s="52"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="49"/>
+      <c r="C5" s="25">
+        <v>43178</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="29">
         <v>95</v>
       </c>
-      <c r="H5" s="41"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="35"/>
-      <c r="C6" s="36">
+      <c r="H5" s="48"/>
+      <c r="J5" s="18">
+        <v>3</v>
+      </c>
+      <c r="K5" s="25">
+        <v>43178</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="21"/>
+      <c r="N5" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="29"/>
+      <c r="P5" s="52"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="49"/>
+      <c r="C6" s="25">
         <v>43180</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="31">
         <v>120</v>
       </c>
-      <c r="H6" s="41"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="35"/>
-      <c r="C7" s="36">
+      <c r="H6" s="48"/>
+      <c r="J6" s="18">
+        <v>4</v>
+      </c>
+      <c r="K6" s="25">
+        <v>43180</v>
+      </c>
+      <c r="L6" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="27"/>
+      <c r="N6" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="31"/>
+      <c r="P6" s="52"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="49"/>
+      <c r="C7" s="25">
         <v>43181</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="31">
         <v>60</v>
       </c>
-      <c r="H7" s="41"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="36">
+      <c r="H7" s="48"/>
+      <c r="J7" s="18">
+        <v>5</v>
+      </c>
+      <c r="K7" s="25">
         <v>43181</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="L7" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="27"/>
+      <c r="N7" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="31"/>
+      <c r="P7" s="52"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="49"/>
+      <c r="C8" s="25">
+        <v>43181</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="31">
         <v>110</v>
       </c>
-      <c r="H8" s="41"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
-      <c r="C9" s="36">
+      <c r="H8" s="48"/>
+      <c r="J8" s="18">
+        <v>6</v>
+      </c>
+      <c r="K8" s="25">
+        <v>43181</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="27"/>
+      <c r="N8" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O8" s="31"/>
+      <c r="P8" s="52"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="49"/>
+      <c r="C9" s="25">
         <v>43182</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="43">
+      <c r="F9" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="31">
         <v>180</v>
       </c>
-      <c r="H9" s="41"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="36">
+      <c r="H9" s="48"/>
+      <c r="J9" s="18">
+        <v>7</v>
+      </c>
+      <c r="K9" s="25">
         <v>43182</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="L9" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="27"/>
+      <c r="N9" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" s="31"/>
+      <c r="P9" s="52"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="49"/>
+      <c r="C10" s="25">
+        <v>43182</v>
+      </c>
+      <c r="D10" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="43">
+      <c r="F10" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="31">
         <v>120</v>
       </c>
-      <c r="H10" s="41"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="35">
+      <c r="H10" s="48"/>
+      <c r="J10" s="18">
+        <v>8</v>
+      </c>
+      <c r="K10" s="25">
+        <v>43182</v>
+      </c>
+      <c r="L10" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="27"/>
+      <c r="N10" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" s="31"/>
+      <c r="P10" s="52"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="49">
         <v>3</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="25">
         <v>43191</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="43">
+      <c r="G11" s="31">
         <v>120</v>
       </c>
-      <c r="H11" s="41">
+      <c r="H11" s="48">
         <f>SUM(G11:G13)</f>
         <v>420</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="35"/>
-      <c r="C12" s="36">
+      <c r="J11" s="18">
+        <v>9</v>
+      </c>
+      <c r="K11" s="25">
+        <v>43191</v>
+      </c>
+      <c r="L11" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="27"/>
+      <c r="N11" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="31"/>
+      <c r="P11" s="52"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="49"/>
+      <c r="C12" s="25">
         <v>43192</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="43">
+      <c r="F12" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="31">
         <v>120</v>
       </c>
-      <c r="H12" s="41"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="35"/>
-      <c r="C13" s="36">
+      <c r="H12" s="48"/>
+      <c r="J12" s="18">
+        <v>10</v>
+      </c>
+      <c r="K12" s="25">
+        <v>43192</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="27"/>
+      <c r="N12" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O12" s="31"/>
+      <c r="P12" s="52"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="49"/>
+      <c r="C13" s="25">
         <v>43193</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="43">
+      <c r="G13" s="31">
         <v>180</v>
       </c>
-      <c r="H13" s="41"/>
-    </row>
-    <row r="14" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="44">
+      <c r="H13" s="48"/>
+      <c r="J13" s="18">
+        <v>11</v>
+      </c>
+      <c r="K13" s="25">
+        <v>43193</v>
+      </c>
+      <c r="L13" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13" s="27"/>
+      <c r="N13" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="O13" s="31"/>
+      <c r="P13" s="52"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="49">
         <v>4</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="25">
         <v>43203</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="49">
+      <c r="F14" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="31">
         <v>120</v>
       </c>
-      <c r="H14" s="50"/>
+      <c r="H14" s="36"/>
+      <c r="J14" s="18">
+        <v>12</v>
+      </c>
+      <c r="K14" s="25">
+        <v>43203</v>
+      </c>
+      <c r="L14" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="27"/>
+      <c r="N14" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="O14" s="31"/>
+      <c r="P14" s="36"/>
+    </row>
+    <row r="15" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="50"/>
+      <c r="C15" s="32">
+        <v>43207</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="51">
+        <v>190</v>
+      </c>
+      <c r="H15" s="37"/>
+      <c r="J15" s="53">
+        <v>13</v>
+      </c>
+      <c r="K15" s="32">
+        <v>43207</v>
+      </c>
+      <c r="L15" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" s="34"/>
+      <c r="N15" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" s="51"/>
+      <c r="P15" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="H4:H10"/>
     <mergeCell ref="H11:H13"/>
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove the Use case "Import the timetable".
</commit_message>
<xml_diff>
--- a/Change_history.xlsx
+++ b/Change_history.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>Revision</t>
   </si>
@@ -204,6 +204,10 @@
   </si>
   <si>
     <t>19:00 - 20:40</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:30 - 20:10</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -271,7 +275,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -557,11 +561,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -652,44 +695,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -699,6 +706,60 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1022,107 +1083,107 @@
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="38">
+      <c r="B6" s="43">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="47">
         <v>43182</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="38"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="43"/>
+      <c r="D7" s="48"/>
     </row>
     <row r="8" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="38"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="43"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="38"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="48"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="43"/>
+      <c r="D10" s="48"/>
     </row>
     <row r="11" spans="2:5" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="44"/>
+      <c r="D11" s="49"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="38">
+      <c r="B12" s="43">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="51">
         <v>43193</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="38"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="47"/>
+      <c r="D13" s="52"/>
     </row>
     <row r="14" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="45"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="47"/>
+      <c r="D14" s="52"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="38">
+      <c r="B15" s="43">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="45">
         <v>43203</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="40"/>
+      <c r="D16" s="45"/>
     </row>
     <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="38"/>
+      <c r="B17" s="43"/>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="40"/>
+      <c r="D17" s="45"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="39"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="41"/>
+      <c r="D18" s="46"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
@@ -1146,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P17"/>
+  <dimension ref="B1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1172,25 +1233,25 @@
   <sheetData>
     <row r="1" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="59" t="s">
         <v>39</v>
       </c>
       <c r="J2" s="14" t="s">
@@ -1216,25 +1277,25 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18">
+      <c r="B3" s="60">
         <v>1</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="25">
         <v>43166</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="23">
+      <c r="F3" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="29">
         <v>60</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="38">
         <v>60</v>
       </c>
       <c r="J3" s="18">
@@ -1254,7 +1315,7 @@
       <c r="P3" s="24"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="49">
+      <c r="B4" s="54">
         <v>2</v>
       </c>
       <c r="C4" s="25">
@@ -1272,7 +1333,7 @@
       <c r="G4" s="29">
         <v>105</v>
       </c>
-      <c r="H4" s="48">
+      <c r="H4" s="53">
         <f>SUM(G4:G10)</f>
         <v>790</v>
       </c>
@@ -1290,10 +1351,10 @@
         <v>40</v>
       </c>
       <c r="O4" s="29"/>
-      <c r="P4" s="52"/>
+      <c r="P4" s="40"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="49"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="25">
         <v>43178</v>
       </c>
@@ -1309,7 +1370,7 @@
       <c r="G5" s="29">
         <v>95</v>
       </c>
-      <c r="H5" s="48"/>
+      <c r="H5" s="53"/>
       <c r="J5" s="18">
         <v>3</v>
       </c>
@@ -1324,10 +1385,10 @@
         <v>40</v>
       </c>
       <c r="O5" s="29"/>
-      <c r="P5" s="52"/>
+      <c r="P5" s="40"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="49"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="25">
         <v>43180</v>
       </c>
@@ -1343,7 +1404,7 @@
       <c r="G6" s="31">
         <v>120</v>
       </c>
-      <c r="H6" s="48"/>
+      <c r="H6" s="53"/>
       <c r="J6" s="18">
         <v>4</v>
       </c>
@@ -1358,10 +1419,10 @@
         <v>40</v>
       </c>
       <c r="O6" s="31"/>
-      <c r="P6" s="52"/>
+      <c r="P6" s="40"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="49"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="25">
         <v>43181</v>
       </c>
@@ -1377,7 +1438,7 @@
       <c r="G7" s="31">
         <v>60</v>
       </c>
-      <c r="H7" s="48"/>
+      <c r="H7" s="53"/>
       <c r="J7" s="18">
         <v>5</v>
       </c>
@@ -1392,10 +1453,10 @@
         <v>40</v>
       </c>
       <c r="O7" s="31"/>
-      <c r="P7" s="52"/>
+      <c r="P7" s="40"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="49"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="25">
         <v>43181</v>
       </c>
@@ -1411,7 +1472,7 @@
       <c r="G8" s="31">
         <v>110</v>
       </c>
-      <c r="H8" s="48"/>
+      <c r="H8" s="53"/>
       <c r="J8" s="18">
         <v>6</v>
       </c>
@@ -1426,10 +1487,10 @@
         <v>40</v>
       </c>
       <c r="O8" s="31"/>
-      <c r="P8" s="52"/>
+      <c r="P8" s="40"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="49"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="25">
         <v>43182</v>
       </c>
@@ -1445,7 +1506,7 @@
       <c r="G9" s="31">
         <v>180</v>
       </c>
-      <c r="H9" s="48"/>
+      <c r="H9" s="53"/>
       <c r="J9" s="18">
         <v>7</v>
       </c>
@@ -1460,10 +1521,10 @@
         <v>40</v>
       </c>
       <c r="O9" s="31"/>
-      <c r="P9" s="52"/>
+      <c r="P9" s="40"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="49"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="25">
         <v>43182</v>
       </c>
@@ -1479,7 +1540,7 @@
       <c r="G10" s="31">
         <v>120</v>
       </c>
-      <c r="H10" s="48"/>
+      <c r="H10" s="53"/>
       <c r="J10" s="18">
         <v>8</v>
       </c>
@@ -1494,10 +1555,10 @@
         <v>40</v>
       </c>
       <c r="O10" s="31"/>
-      <c r="P10" s="52"/>
+      <c r="P10" s="40"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="49">
+      <c r="B11" s="54">
         <v>3</v>
       </c>
       <c r="C11" s="25">
@@ -1515,7 +1576,7 @@
       <c r="G11" s="31">
         <v>120</v>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="53">
         <f>SUM(G11:G13)</f>
         <v>420</v>
       </c>
@@ -1533,10 +1594,10 @@
         <v>40</v>
       </c>
       <c r="O11" s="31"/>
-      <c r="P11" s="52"/>
+      <c r="P11" s="40"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="49"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="25">
         <v>43192</v>
       </c>
@@ -1552,7 +1613,7 @@
       <c r="G12" s="31">
         <v>120</v>
       </c>
-      <c r="H12" s="48"/>
+      <c r="H12" s="53"/>
       <c r="J12" s="18">
         <v>10</v>
       </c>
@@ -1567,10 +1628,10 @@
         <v>40</v>
       </c>
       <c r="O12" s="31"/>
-      <c r="P12" s="52"/>
+      <c r="P12" s="40"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="49"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="25">
         <v>43193</v>
       </c>
@@ -1586,7 +1647,7 @@
       <c r="G13" s="31">
         <v>180</v>
       </c>
-      <c r="H13" s="48"/>
+      <c r="H13" s="53"/>
       <c r="J13" s="18">
         <v>11</v>
       </c>
@@ -1601,10 +1662,10 @@
         <v>42</v>
       </c>
       <c r="O13" s="31"/>
-      <c r="P13" s="52"/>
+      <c r="P13" s="40"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="49">
+      <c r="B14" s="54">
         <v>4</v>
       </c>
       <c r="C14" s="25">
@@ -1640,7 +1701,7 @@
       <c r="P14" s="36"/>
     </row>
     <row r="15" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="49"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="25">
         <v>43207</v>
       </c>
@@ -1656,8 +1717,8 @@
       <c r="G15" s="31">
         <v>190</v>
       </c>
-      <c r="H15" s="54"/>
-      <c r="J15" s="53">
+      <c r="H15" s="42"/>
+      <c r="J15" s="41">
         <v>13</v>
       </c>
       <c r="K15" s="32">
@@ -1670,11 +1731,11 @@
       <c r="N15" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="51"/>
+      <c r="O15" s="39"/>
       <c r="P15" s="37"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="49"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="25">
         <v>43208</v>
       </c>
@@ -1690,26 +1751,45 @@
       <c r="G16" s="31">
         <v>30</v>
       </c>
-      <c r="H16" s="54"/>
-    </row>
-    <row r="17" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="50"/>
-      <c r="C17" s="32">
+      <c r="H16" s="42"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="54"/>
+      <c r="C17" s="25">
         <v>43208</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="51">
+      <c r="F17" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="31">
         <v>100</v>
       </c>
-      <c r="H17" s="37"/>
+      <c r="H17" s="42"/>
+    </row>
+    <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="55"/>
+      <c r="C18" s="32">
+        <v>43214</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="39">
+        <v>100</v>
+      </c>
+      <c r="H18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1717,7 +1797,7 @@
     <mergeCell ref="H11:H13"/>
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B14:B18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commit doc and server->findEvent and deleteEvent
</commit_message>
<xml_diff>
--- a/Change_history.xlsx
+++ b/Change_history.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
   <si>
     <t>Revision</t>
   </si>
@@ -208,6 +208,10 @@
   </si>
   <si>
     <t>18:30 - 20:10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>19:00 ~ 20:40</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -604,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -702,10 +706,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -745,19 +761,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1083,107 +1103,107 @@
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="43">
+      <c r="B6" s="47">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="51">
         <v>43182</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="48"/>
+      <c r="D7" s="52"/>
     </row>
     <row r="8" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="43"/>
+      <c r="B8" s="47"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="52"/>
     </row>
     <row r="9" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="48"/>
+      <c r="D9" s="52"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="48"/>
+      <c r="D10" s="52"/>
     </row>
     <row r="11" spans="2:5" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="49"/>
+      <c r="D11" s="53"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="43">
+      <c r="B12" s="47">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="55">
         <v>43193</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="43"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="52"/>
+      <c r="D13" s="56"/>
     </row>
     <row r="14" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="50"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="52"/>
+      <c r="D14" s="56"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="43">
+      <c r="B15" s="47">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="45">
+      <c r="D15" s="49">
         <v>43203</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="43"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="45"/>
+      <c r="D16" s="49"/>
     </row>
     <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="43"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="45"/>
+      <c r="D17" s="49"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="44"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="46"/>
+      <c r="D18" s="50"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
@@ -1210,7 +1230,7 @@
   <dimension ref="B1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1233,25 +1253,25 @@
   <sheetData>
     <row r="1" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="45" t="s">
         <v>39</v>
       </c>
       <c r="J2" s="14" t="s">
@@ -1277,7 +1297,7 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="60">
+      <c r="B3" s="46">
         <v>1</v>
       </c>
       <c r="C3" s="25">
@@ -1315,7 +1335,7 @@
       <c r="P3" s="24"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="54">
+      <c r="B4" s="58">
         <v>2</v>
       </c>
       <c r="C4" s="25">
@@ -1333,7 +1353,7 @@
       <c r="G4" s="29">
         <v>105</v>
       </c>
-      <c r="H4" s="53">
+      <c r="H4" s="57">
         <f>SUM(G4:G10)</f>
         <v>790</v>
       </c>
@@ -1354,7 +1374,7 @@
       <c r="P4" s="40"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="54"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="25">
         <v>43178</v>
       </c>
@@ -1370,7 +1390,7 @@
       <c r="G5" s="29">
         <v>95</v>
       </c>
-      <c r="H5" s="53"/>
+      <c r="H5" s="57"/>
       <c r="J5" s="18">
         <v>3</v>
       </c>
@@ -1388,7 +1408,7 @@
       <c r="P5" s="40"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="54"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="25">
         <v>43180</v>
       </c>
@@ -1404,7 +1424,7 @@
       <c r="G6" s="31">
         <v>120</v>
       </c>
-      <c r="H6" s="53"/>
+      <c r="H6" s="57"/>
       <c r="J6" s="18">
         <v>4</v>
       </c>
@@ -1422,7 +1442,7 @@
       <c r="P6" s="40"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="54"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="25">
         <v>43181</v>
       </c>
@@ -1438,7 +1458,7 @@
       <c r="G7" s="31">
         <v>60</v>
       </c>
-      <c r="H7" s="53"/>
+      <c r="H7" s="57"/>
       <c r="J7" s="18">
         <v>5</v>
       </c>
@@ -1456,7 +1476,7 @@
       <c r="P7" s="40"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="54"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="25">
         <v>43181</v>
       </c>
@@ -1472,7 +1492,7 @@
       <c r="G8" s="31">
         <v>110</v>
       </c>
-      <c r="H8" s="53"/>
+      <c r="H8" s="57"/>
       <c r="J8" s="18">
         <v>6</v>
       </c>
@@ -1490,7 +1510,7 @@
       <c r="P8" s="40"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="25">
         <v>43182</v>
       </c>
@@ -1506,7 +1526,7 @@
       <c r="G9" s="31">
         <v>180</v>
       </c>
-      <c r="H9" s="53"/>
+      <c r="H9" s="57"/>
       <c r="J9" s="18">
         <v>7</v>
       </c>
@@ -1524,7 +1544,7 @@
       <c r="P9" s="40"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="54"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="25">
         <v>43182</v>
       </c>
@@ -1540,7 +1560,7 @@
       <c r="G10" s="31">
         <v>120</v>
       </c>
-      <c r="H10" s="53"/>
+      <c r="H10" s="57"/>
       <c r="J10" s="18">
         <v>8</v>
       </c>
@@ -1558,7 +1578,7 @@
       <c r="P10" s="40"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="54">
+      <c r="B11" s="58">
         <v>3</v>
       </c>
       <c r="C11" s="25">
@@ -1576,7 +1596,7 @@
       <c r="G11" s="31">
         <v>120</v>
       </c>
-      <c r="H11" s="53">
+      <c r="H11" s="57">
         <f>SUM(G11:G13)</f>
         <v>420</v>
       </c>
@@ -1597,7 +1617,7 @@
       <c r="P11" s="40"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="54"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="25">
         <v>43192</v>
       </c>
@@ -1613,7 +1633,7 @@
       <c r="G12" s="31">
         <v>120</v>
       </c>
-      <c r="H12" s="53"/>
+      <c r="H12" s="57"/>
       <c r="J12" s="18">
         <v>10</v>
       </c>
@@ -1631,7 +1651,7 @@
       <c r="P12" s="40"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="54"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="25">
         <v>43193</v>
       </c>
@@ -1647,7 +1667,7 @@
       <c r="G13" s="31">
         <v>180</v>
       </c>
-      <c r="H13" s="53"/>
+      <c r="H13" s="57"/>
       <c r="J13" s="18">
         <v>11</v>
       </c>
@@ -1665,7 +1685,7 @@
       <c r="P13" s="40"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="54">
+      <c r="B14" s="58">
         <v>4</v>
       </c>
       <c r="C14" s="25">
@@ -1700,8 +1720,8 @@
       <c r="O14" s="31"/>
       <c r="P14" s="36"/>
     </row>
-    <row r="15" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="54"/>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="58"/>
       <c r="C15" s="25">
         <v>43207</v>
       </c>
@@ -1717,25 +1737,25 @@
       <c r="G15" s="31">
         <v>190</v>
       </c>
-      <c r="H15" s="42"/>
-      <c r="J15" s="41">
+      <c r="H15" s="41"/>
+      <c r="J15" s="60">
         <v>13</v>
       </c>
-      <c r="K15" s="32">
+      <c r="K15" s="61">
         <v>43207</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="L15" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="34"/>
-      <c r="N15" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="O15" s="39"/>
-      <c r="P15" s="37"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="54"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" s="65"/>
+      <c r="P15" s="66"/>
+    </row>
+    <row r="16" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="58"/>
       <c r="C16" s="25">
         <v>43208</v>
       </c>
@@ -1751,10 +1771,25 @@
       <c r="G16" s="31">
         <v>30</v>
       </c>
-      <c r="H16" s="42"/>
+      <c r="H16" s="41"/>
+      <c r="J16" s="68">
+        <v>14</v>
+      </c>
+      <c r="K16" s="32">
+        <v>43215</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="M16" s="67"/>
+      <c r="N16" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="O16" s="67"/>
+      <c r="P16" s="37"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="25">
         <v>43208</v>
       </c>
@@ -1770,10 +1805,10 @@
       <c r="G17" s="31">
         <v>100</v>
       </c>
-      <c r="H17" s="42"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="55"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="32">
         <v>43214</v>
       </c>

</xml_diff>

<commit_message>
finish homework4 sequence_diagram modify class_diagram
</commit_message>
<xml_diff>
--- a/Change_history.xlsx
+++ b/Change_history.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
   <si>
     <t>Revision</t>
   </si>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>19:00 ~ 20:40</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write the homework 4.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:30 - 21:01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>19:00 - 21:15</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -279,7 +291,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -604,11 +616,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -699,67 +748,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -778,6 +787,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1103,107 +1169,107 @@
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="47">
+      <c r="B6" s="55">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="59">
         <v>43182</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="52"/>
+      <c r="D7" s="60"/>
     </row>
     <row r="8" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="47"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="52"/>
+      <c r="D8" s="60"/>
     </row>
     <row r="9" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="47"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="52"/>
+      <c r="D9" s="60"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="52"/>
+      <c r="D10" s="60"/>
     </row>
     <row r="11" spans="2:5" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="53"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="47">
+      <c r="B12" s="55">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="63">
         <v>43193</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="56"/>
+      <c r="D13" s="64"/>
     </row>
     <row r="14" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="54"/>
+      <c r="B14" s="62"/>
       <c r="C14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="56"/>
+      <c r="D14" s="64"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="47">
+      <c r="B15" s="55">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="49">
+      <c r="D15" s="57">
         <v>43203</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="49"/>
+      <c r="D16" s="57"/>
     </row>
     <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="D17" s="57"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="48"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="50"/>
+      <c r="D18" s="58"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
@@ -1227,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P18"/>
+  <dimension ref="B1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1253,25 +1319,25 @@
   <sheetData>
     <row r="1" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="43" t="s">
         <v>39</v>
       </c>
       <c r="J2" s="14" t="s">
@@ -1297,7 +1363,7 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="46">
+      <c r="B3" s="44">
         <v>1</v>
       </c>
       <c r="C3" s="25">
@@ -1315,7 +1381,7 @@
       <c r="G3" s="29">
         <v>60</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="45">
         <v>60</v>
       </c>
       <c r="J3" s="18">
@@ -1335,7 +1401,7 @@
       <c r="P3" s="24"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="58">
+      <c r="B4" s="66">
         <v>2</v>
       </c>
       <c r="C4" s="25">
@@ -1353,7 +1419,7 @@
       <c r="G4" s="29">
         <v>105</v>
       </c>
-      <c r="H4" s="57">
+      <c r="H4" s="65">
         <f>SUM(G4:G10)</f>
         <v>790</v>
       </c>
@@ -1371,10 +1437,10 @@
         <v>40</v>
       </c>
       <c r="O4" s="29"/>
-      <c r="P4" s="40"/>
+      <c r="P4" s="39"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="58"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="25">
         <v>43178</v>
       </c>
@@ -1390,7 +1456,7 @@
       <c r="G5" s="29">
         <v>95</v>
       </c>
-      <c r="H5" s="57"/>
+      <c r="H5" s="65"/>
       <c r="J5" s="18">
         <v>3</v>
       </c>
@@ -1405,10 +1471,10 @@
         <v>40</v>
       </c>
       <c r="O5" s="29"/>
-      <c r="P5" s="40"/>
+      <c r="P5" s="39"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="58"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="25">
         <v>43180</v>
       </c>
@@ -1424,7 +1490,7 @@
       <c r="G6" s="31">
         <v>120</v>
       </c>
-      <c r="H6" s="57"/>
+      <c r="H6" s="65"/>
       <c r="J6" s="18">
         <v>4</v>
       </c>
@@ -1439,10 +1505,10 @@
         <v>40</v>
       </c>
       <c r="O6" s="31"/>
-      <c r="P6" s="40"/>
+      <c r="P6" s="39"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="58"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="25">
         <v>43181</v>
       </c>
@@ -1458,7 +1524,7 @@
       <c r="G7" s="31">
         <v>60</v>
       </c>
-      <c r="H7" s="57"/>
+      <c r="H7" s="65"/>
       <c r="J7" s="18">
         <v>5</v>
       </c>
@@ -1473,10 +1539,10 @@
         <v>40</v>
       </c>
       <c r="O7" s="31"/>
-      <c r="P7" s="40"/>
+      <c r="P7" s="39"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="58"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="25">
         <v>43181</v>
       </c>
@@ -1492,7 +1558,7 @@
       <c r="G8" s="31">
         <v>110</v>
       </c>
-      <c r="H8" s="57"/>
+      <c r="H8" s="65"/>
       <c r="J8" s="18">
         <v>6</v>
       </c>
@@ -1507,10 +1573,10 @@
         <v>40</v>
       </c>
       <c r="O8" s="31"/>
-      <c r="P8" s="40"/>
+      <c r="P8" s="39"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="25">
         <v>43182</v>
       </c>
@@ -1526,7 +1592,7 @@
       <c r="G9" s="31">
         <v>180</v>
       </c>
-      <c r="H9" s="57"/>
+      <c r="H9" s="65"/>
       <c r="J9" s="18">
         <v>7</v>
       </c>
@@ -1541,10 +1607,10 @@
         <v>40</v>
       </c>
       <c r="O9" s="31"/>
-      <c r="P9" s="40"/>
+      <c r="P9" s="39"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="58"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="25">
         <v>43182</v>
       </c>
@@ -1560,7 +1626,7 @@
       <c r="G10" s="31">
         <v>120</v>
       </c>
-      <c r="H10" s="57"/>
+      <c r="H10" s="65"/>
       <c r="J10" s="18">
         <v>8</v>
       </c>
@@ -1575,10 +1641,10 @@
         <v>40</v>
       </c>
       <c r="O10" s="31"/>
-      <c r="P10" s="40"/>
+      <c r="P10" s="39"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="58">
+      <c r="B11" s="66">
         <v>3</v>
       </c>
       <c r="C11" s="25">
@@ -1596,7 +1662,7 @@
       <c r="G11" s="31">
         <v>120</v>
       </c>
-      <c r="H11" s="57">
+      <c r="H11" s="65">
         <f>SUM(G11:G13)</f>
         <v>420</v>
       </c>
@@ -1614,10 +1680,10 @@
         <v>40</v>
       </c>
       <c r="O11" s="31"/>
-      <c r="P11" s="40"/>
+      <c r="P11" s="39"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="58"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="25">
         <v>43192</v>
       </c>
@@ -1633,7 +1699,7 @@
       <c r="G12" s="31">
         <v>120</v>
       </c>
-      <c r="H12" s="57"/>
+      <c r="H12" s="65"/>
       <c r="J12" s="18">
         <v>10</v>
       </c>
@@ -1648,10 +1714,10 @@
         <v>40</v>
       </c>
       <c r="O12" s="31"/>
-      <c r="P12" s="40"/>
+      <c r="P12" s="39"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="25">
         <v>43193</v>
       </c>
@@ -1667,7 +1733,7 @@
       <c r="G13" s="31">
         <v>180</v>
       </c>
-      <c r="H13" s="57"/>
+      <c r="H13" s="65"/>
       <c r="J13" s="18">
         <v>11</v>
       </c>
@@ -1682,10 +1748,10 @@
         <v>42</v>
       </c>
       <c r="O13" s="31"/>
-      <c r="P13" s="40"/>
+      <c r="P13" s="39"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="58">
+      <c r="B14" s="67">
         <v>4</v>
       </c>
       <c r="C14" s="25">
@@ -1703,7 +1769,10 @@
       <c r="G14" s="31">
         <v>120</v>
       </c>
-      <c r="H14" s="36"/>
+      <c r="H14" s="70">
+        <f>SUM(G14:G20)</f>
+        <v>826</v>
+      </c>
       <c r="J14" s="18">
         <v>12</v>
       </c>
@@ -1721,7 +1790,7 @@
       <c r="P14" s="36"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="58"/>
+      <c r="B15" s="68"/>
       <c r="C15" s="25">
         <v>43207</v>
       </c>
@@ -1737,25 +1806,25 @@
       <c r="G15" s="31">
         <v>190</v>
       </c>
-      <c r="H15" s="41"/>
-      <c r="J15" s="60">
+      <c r="H15" s="71"/>
+      <c r="J15" s="46">
         <v>13</v>
       </c>
-      <c r="K15" s="61">
+      <c r="K15" s="47">
         <v>43207</v>
       </c>
-      <c r="L15" s="62" t="s">
+      <c r="L15" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="63"/>
-      <c r="N15" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="O15" s="65"/>
-      <c r="P15" s="66"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" s="51"/>
+      <c r="P15" s="52"/>
     </row>
     <row r="16" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="25">
         <v>43208</v>
       </c>
@@ -1771,8 +1840,8 @@
       <c r="G16" s="31">
         <v>30</v>
       </c>
-      <c r="H16" s="41"/>
-      <c r="J16" s="68">
+      <c r="H16" s="71"/>
+      <c r="J16" s="54">
         <v>14</v>
       </c>
       <c r="K16" s="32">
@@ -1781,15 +1850,15 @@
       <c r="L16" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="M16" s="67"/>
+      <c r="M16" s="53"/>
       <c r="N16" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="O16" s="67"/>
+      <c r="O16" s="53"/>
       <c r="P16" s="37"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="58"/>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="68"/>
       <c r="C17" s="25">
         <v>43208</v>
       </c>
@@ -1805,34 +1874,183 @@
       <c r="G17" s="31">
         <v>100</v>
       </c>
-      <c r="H17" s="41"/>
-    </row>
-    <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="59"/>
-      <c r="C18" s="32">
+      <c r="H17" s="71"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="68"/>
+      <c r="C18" s="47">
         <v>43214</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="39">
+      <c r="F18" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="51">
         <v>100</v>
       </c>
-      <c r="H18" s="37"/>
+      <c r="H18" s="71"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B19" s="68"/>
+      <c r="C19" s="25">
+        <v>43222</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="31">
+        <v>135</v>
+      </c>
+      <c r="H19" s="71"/>
+    </row>
+    <row r="20" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="69"/>
+      <c r="C20" s="32">
+        <v>43223</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="38">
+        <v>151</v>
+      </c>
+      <c r="H20" s="72"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="O26" s="3"/>
+      <c r="P26" s="73"/>
+      <c r="Q26" s="73"/>
+      <c r="R26" s="73"/>
+      <c r="S26" s="73"/>
+      <c r="T26" s="73"/>
+      <c r="U26" s="73"/>
+      <c r="V26" s="73"/>
+      <c r="W26" s="3"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="O27" s="3"/>
+      <c r="P27" s="73"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="O28" s="3"/>
+      <c r="P28" s="73"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="O29" s="3"/>
+      <c r="P29" s="73"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="O30" s="3"/>
+      <c r="P30" s="73"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="O31" s="3"/>
+      <c r="P31" s="73"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="O32" s="3"/>
+      <c r="P32" s="73"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+    </row>
+    <row r="33" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+    </row>
+    <row r="34" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="H14:H20"/>
     <mergeCell ref="H4:H10"/>
     <mergeCell ref="H11:H13"/>
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commit doc and diagram and server unit test
</commit_message>
<xml_diff>
--- a/Change_history.xlsx
+++ b/Change_history.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="59">
   <si>
     <t>Revision</t>
   </si>
@@ -224,6 +224,22 @@
   </si>
   <si>
     <t>19:00 - 21:15</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:30 - 22:00</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:00 - 23:00</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>09:00 - 15:00</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write the homework 5.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -767,9 +783,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -789,6 +802,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -819,32 +838,29 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1169,107 +1185,107 @@
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="55">
+      <c r="B6" s="56">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="59">
+      <c r="D6" s="60">
         <v>43182</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="55"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="60"/>
+      <c r="D7" s="61"/>
     </row>
     <row r="8" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="55"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="61"/>
     </row>
     <row r="9" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="55"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="60"/>
+      <c r="D9" s="61"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="55"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="60"/>
+      <c r="D10" s="61"/>
     </row>
     <row r="11" spans="2:5" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="55"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="61"/>
+      <c r="D11" s="62"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="55">
+      <c r="B12" s="56">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="64">
         <v>43193</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="55"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="64"/>
+      <c r="D13" s="65"/>
     </row>
     <row r="14" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="62"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="64"/>
+      <c r="D14" s="65"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="55">
+      <c r="B15" s="56">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="57">
+      <c r="D15" s="58">
         <v>43203</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="55"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="57"/>
+      <c r="D16" s="58"/>
     </row>
     <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="55"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="57"/>
+      <c r="D17" s="58"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="56"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="58"/>
+      <c r="D18" s="59"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
@@ -1295,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1381,7 +1397,7 @@
       <c r="G3" s="29">
         <v>60</v>
       </c>
-      <c r="H3" s="45">
+      <c r="H3" s="54">
         <v>60</v>
       </c>
       <c r="J3" s="18">
@@ -1401,7 +1417,7 @@
       <c r="P3" s="24"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="66">
+      <c r="B4" s="73">
         <v>2</v>
       </c>
       <c r="C4" s="25">
@@ -1419,7 +1435,7 @@
       <c r="G4" s="29">
         <v>105</v>
       </c>
-      <c r="H4" s="65">
+      <c r="H4" s="72">
         <f>SUM(G4:G10)</f>
         <v>790</v>
       </c>
@@ -1440,7 +1456,7 @@
       <c r="P4" s="39"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="66"/>
+      <c r="B5" s="73"/>
       <c r="C5" s="25">
         <v>43178</v>
       </c>
@@ -1456,7 +1472,7 @@
       <c r="G5" s="29">
         <v>95</v>
       </c>
-      <c r="H5" s="65"/>
+      <c r="H5" s="72"/>
       <c r="J5" s="18">
         <v>3</v>
       </c>
@@ -1474,7 +1490,7 @@
       <c r="P5" s="39"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="66"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="25">
         <v>43180</v>
       </c>
@@ -1490,7 +1506,7 @@
       <c r="G6" s="31">
         <v>120</v>
       </c>
-      <c r="H6" s="65"/>
+      <c r="H6" s="72"/>
       <c r="J6" s="18">
         <v>4</v>
       </c>
@@ -1508,7 +1524,7 @@
       <c r="P6" s="39"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="66"/>
+      <c r="B7" s="73"/>
       <c r="C7" s="25">
         <v>43181</v>
       </c>
@@ -1524,7 +1540,7 @@
       <c r="G7" s="31">
         <v>60</v>
       </c>
-      <c r="H7" s="65"/>
+      <c r="H7" s="72"/>
       <c r="J7" s="18">
         <v>5</v>
       </c>
@@ -1542,7 +1558,7 @@
       <c r="P7" s="39"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="66"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="25">
         <v>43181</v>
       </c>
@@ -1558,7 +1574,7 @@
       <c r="G8" s="31">
         <v>110</v>
       </c>
-      <c r="H8" s="65"/>
+      <c r="H8" s="72"/>
       <c r="J8" s="18">
         <v>6</v>
       </c>
@@ -1576,7 +1592,7 @@
       <c r="P8" s="39"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="66"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="25">
         <v>43182</v>
       </c>
@@ -1592,7 +1608,7 @@
       <c r="G9" s="31">
         <v>180</v>
       </c>
-      <c r="H9" s="65"/>
+      <c r="H9" s="72"/>
       <c r="J9" s="18">
         <v>7</v>
       </c>
@@ -1610,7 +1626,7 @@
       <c r="P9" s="39"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="66"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="25">
         <v>43182</v>
       </c>
@@ -1626,7 +1642,7 @@
       <c r="G10" s="31">
         <v>120</v>
       </c>
-      <c r="H10" s="65"/>
+      <c r="H10" s="72"/>
       <c r="J10" s="18">
         <v>8</v>
       </c>
@@ -1644,7 +1660,7 @@
       <c r="P10" s="39"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="66">
+      <c r="B11" s="73">
         <v>3</v>
       </c>
       <c r="C11" s="25">
@@ -1662,7 +1678,7 @@
       <c r="G11" s="31">
         <v>120</v>
       </c>
-      <c r="H11" s="65">
+      <c r="H11" s="72">
         <f>SUM(G11:G13)</f>
         <v>420</v>
       </c>
@@ -1683,7 +1699,7 @@
       <c r="P11" s="39"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="66"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="25">
         <v>43192</v>
       </c>
@@ -1699,7 +1715,7 @@
       <c r="G12" s="31">
         <v>120</v>
       </c>
-      <c r="H12" s="65"/>
+      <c r="H12" s="72"/>
       <c r="J12" s="18">
         <v>10</v>
       </c>
@@ -1717,7 +1733,7 @@
       <c r="P12" s="39"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="66"/>
+      <c r="B13" s="73"/>
       <c r="C13" s="25">
         <v>43193</v>
       </c>
@@ -1733,7 +1749,7 @@
       <c r="G13" s="31">
         <v>180</v>
       </c>
-      <c r="H13" s="65"/>
+      <c r="H13" s="72"/>
       <c r="J13" s="18">
         <v>11</v>
       </c>
@@ -1751,7 +1767,7 @@
       <c r="P13" s="39"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="67">
+      <c r="B14" s="66">
         <v>4</v>
       </c>
       <c r="C14" s="25">
@@ -1769,7 +1785,7 @@
       <c r="G14" s="31">
         <v>120</v>
       </c>
-      <c r="H14" s="70">
+      <c r="H14" s="69">
         <f>SUM(G14:G20)</f>
         <v>826</v>
       </c>
@@ -1790,7 +1806,7 @@
       <c r="P14" s="36"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="68"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="25">
         <v>43207</v>
       </c>
@@ -1806,25 +1822,25 @@
       <c r="G15" s="31">
         <v>190</v>
       </c>
-      <c r="H15" s="71"/>
-      <c r="J15" s="46">
+      <c r="H15" s="70"/>
+      <c r="J15" s="45">
         <v>13</v>
       </c>
-      <c r="K15" s="47">
+      <c r="K15" s="46">
         <v>43207</v>
       </c>
-      <c r="L15" s="48" t="s">
+      <c r="L15" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="49"/>
-      <c r="N15" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="O15" s="51"/>
-      <c r="P15" s="52"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" s="50"/>
+      <c r="P15" s="51"/>
     </row>
     <row r="16" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="68"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="25">
         <v>43208</v>
       </c>
@@ -1840,8 +1856,8 @@
       <c r="G16" s="31">
         <v>30</v>
       </c>
-      <c r="H16" s="71"/>
-      <c r="J16" s="54">
+      <c r="H16" s="70"/>
+      <c r="J16" s="53">
         <v>14</v>
       </c>
       <c r="K16" s="32">
@@ -1850,15 +1866,15 @@
       <c r="L16" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="M16" s="53"/>
+      <c r="M16" s="52"/>
       <c r="N16" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="O16" s="53"/>
+      <c r="O16" s="52"/>
       <c r="P16" s="37"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="68"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="25">
         <v>43208</v>
       </c>
@@ -1874,29 +1890,29 @@
       <c r="G17" s="31">
         <v>100</v>
       </c>
-      <c r="H17" s="71"/>
+      <c r="H17" s="70"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="68"/>
-      <c r="C18" s="47">
+      <c r="B18" s="67"/>
+      <c r="C18" s="46">
         <v>43214</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="49" t="s">
+      <c r="E18" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="51">
+      <c r="F18" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="50">
         <v>100</v>
       </c>
-      <c r="H18" s="71"/>
+      <c r="H18" s="70"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B19" s="68"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="25">
         <v>43222</v>
       </c>
@@ -1912,26 +1928,87 @@
       <c r="G19" s="31">
         <v>135</v>
       </c>
-      <c r="H19" s="71"/>
-    </row>
-    <row r="20" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="69"/>
-      <c r="C20" s="32">
+      <c r="H19" s="70"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B20" s="67"/>
+      <c r="C20" s="46">
         <v>43223</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="38">
+      <c r="F20" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="50">
         <v>151</v>
       </c>
-      <c r="H20" s="72"/>
+      <c r="H20" s="70"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B21" s="66">
+        <v>5</v>
+      </c>
+      <c r="C21" s="25">
+        <v>43229</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="31">
+        <v>210</v>
+      </c>
+      <c r="H21" s="69">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B22" s="67"/>
+      <c r="C22" s="25">
+        <v>43230</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="31">
+        <v>360</v>
+      </c>
+      <c r="H22" s="70"/>
+    </row>
+    <row r="23" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="68"/>
+      <c r="C23" s="32">
+        <v>43231</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="38">
+        <v>360</v>
+      </c>
+      <c r="H23" s="71"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="O25" s="3"/>
@@ -1946,18 +2023,18 @@
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="O26" s="3"/>
-      <c r="P26" s="73"/>
-      <c r="Q26" s="73"/>
-      <c r="R26" s="73"/>
-      <c r="S26" s="73"/>
-      <c r="T26" s="73"/>
-      <c r="U26" s="73"/>
-      <c r="V26" s="73"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="55"/>
+      <c r="U26" s="55"/>
+      <c r="V26" s="55"/>
       <c r="W26" s="3"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="O27" s="3"/>
-      <c r="P27" s="73"/>
+      <c r="P27" s="55"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
@@ -1968,7 +2045,7 @@
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="O28" s="3"/>
-      <c r="P28" s="73"/>
+      <c r="P28" s="55"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
@@ -1979,7 +2056,7 @@
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="O29" s="3"/>
-      <c r="P29" s="73"/>
+      <c r="P29" s="55"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
@@ -1990,7 +2067,7 @@
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="O30" s="3"/>
-      <c r="P30" s="73"/>
+      <c r="P30" s="55"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
@@ -2001,7 +2078,7 @@
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="O31" s="3"/>
-      <c r="P31" s="73"/>
+      <c r="P31" s="55"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
@@ -2012,7 +2089,7 @@
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="O32" s="3"/>
-      <c r="P32" s="73"/>
+      <c r="P32" s="55"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
@@ -2044,7 +2121,9 @@
       <c r="W34" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="B21:B23"/>
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="H14:H20"/>
     <mergeCell ref="H4:H10"/>

</xml_diff>

<commit_message>
commit document and pic
</commit_message>
<xml_diff>
--- a/Change_history.xlsx
+++ b/Change_history.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="65">
   <si>
     <t>Revision</t>
   </si>
@@ -252,6 +252,18 @@
   </si>
   <si>
     <t>鍾承翰、楊子冊、吳彥銘</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write the homework 7.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>09:00 - 12:00</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:00 - 20:00</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -319,7 +331,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -655,11 +667,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -794,6 +850,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -824,28 +886,32 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1171,107 +1237,107 @@
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="56">
+      <c r="B6" s="58">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="62">
         <v>43182</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="56"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="61"/>
+      <c r="D7" s="63"/>
     </row>
     <row r="8" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="56"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="61"/>
+      <c r="D8" s="63"/>
     </row>
     <row r="9" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="56"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="61"/>
+      <c r="D9" s="63"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="56"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="61"/>
+      <c r="D10" s="63"/>
     </row>
     <row r="11" spans="2:5" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="56"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="62"/>
+      <c r="D11" s="64"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="56">
+      <c r="B12" s="58">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="66">
         <v>43193</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="56"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="65"/>
+      <c r="D13" s="67"/>
     </row>
     <row r="14" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="63"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="65"/>
+      <c r="D14" s="67"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="56">
+      <c r="B15" s="58">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="60">
         <v>43203</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="56"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="58"/>
+      <c r="D16" s="60"/>
     </row>
     <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="56"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="58"/>
+      <c r="D17" s="60"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="57"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="59"/>
+      <c r="D18" s="61"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
@@ -1298,7 +1364,7 @@
   <dimension ref="B1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="B2" sqref="B2:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1403,7 +1469,7 @@
       <c r="P3" s="24"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="71">
+      <c r="B4" s="69">
         <v>2</v>
       </c>
       <c r="C4" s="25">
@@ -1421,7 +1487,7 @@
       <c r="G4" s="29">
         <v>105</v>
       </c>
-      <c r="H4" s="70">
+      <c r="H4" s="68">
         <f>SUM(G4:G10)</f>
         <v>790</v>
       </c>
@@ -1442,7 +1508,7 @@
       <c r="P4" s="39"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="71"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="25">
         <v>43178</v>
       </c>
@@ -1458,7 +1524,7 @@
       <c r="G5" s="29">
         <v>95</v>
       </c>
-      <c r="H5" s="70"/>
+      <c r="H5" s="68"/>
       <c r="J5" s="18">
         <v>3</v>
       </c>
@@ -1476,7 +1542,7 @@
       <c r="P5" s="39"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="71"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="25">
         <v>43180</v>
       </c>
@@ -1492,7 +1558,7 @@
       <c r="G6" s="31">
         <v>120</v>
       </c>
-      <c r="H6" s="70"/>
+      <c r="H6" s="68"/>
       <c r="J6" s="18">
         <v>4</v>
       </c>
@@ -1510,7 +1576,7 @@
       <c r="P6" s="39"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="71"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="25">
         <v>43181</v>
       </c>
@@ -1526,7 +1592,7 @@
       <c r="G7" s="31">
         <v>60</v>
       </c>
-      <c r="H7" s="70"/>
+      <c r="H7" s="68"/>
       <c r="J7" s="18">
         <v>5</v>
       </c>
@@ -1544,7 +1610,7 @@
       <c r="P7" s="39"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="71"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="25">
         <v>43181</v>
       </c>
@@ -1560,7 +1626,7 @@
       <c r="G8" s="31">
         <v>110</v>
       </c>
-      <c r="H8" s="70"/>
+      <c r="H8" s="68"/>
       <c r="J8" s="18">
         <v>6</v>
       </c>
@@ -1578,7 +1644,7 @@
       <c r="P8" s="39"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="71"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="25">
         <v>43182</v>
       </c>
@@ -1594,7 +1660,7 @@
       <c r="G9" s="31">
         <v>180</v>
       </c>
-      <c r="H9" s="70"/>
+      <c r="H9" s="68"/>
       <c r="J9" s="18">
         <v>7</v>
       </c>
@@ -1612,7 +1678,7 @@
       <c r="P9" s="39"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="71"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="25">
         <v>43182</v>
       </c>
@@ -1628,7 +1694,7 @@
       <c r="G10" s="31">
         <v>120</v>
       </c>
-      <c r="H10" s="70"/>
+      <c r="H10" s="68"/>
       <c r="J10" s="18">
         <v>8</v>
       </c>
@@ -1646,7 +1712,7 @@
       <c r="P10" s="39"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="71">
+      <c r="B11" s="69">
         <v>3</v>
       </c>
       <c r="C11" s="25">
@@ -1664,7 +1730,7 @@
       <c r="G11" s="31">
         <v>120</v>
       </c>
-      <c r="H11" s="70">
+      <c r="H11" s="68">
         <f>SUM(G11:G13)</f>
         <v>420</v>
       </c>
@@ -1685,7 +1751,7 @@
       <c r="P11" s="39"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="71"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="25">
         <v>43192</v>
       </c>
@@ -1701,7 +1767,7 @@
       <c r="G12" s="31">
         <v>120</v>
       </c>
-      <c r="H12" s="70"/>
+      <c r="H12" s="68"/>
       <c r="J12" s="18">
         <v>10</v>
       </c>
@@ -1719,7 +1785,7 @@
       <c r="P12" s="39"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="71"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="25">
         <v>43193</v>
       </c>
@@ -1735,7 +1801,7 @@
       <c r="G13" s="31">
         <v>180</v>
       </c>
-      <c r="H13" s="70"/>
+      <c r="H13" s="68"/>
       <c r="J13" s="18">
         <v>11</v>
       </c>
@@ -1753,7 +1819,7 @@
       <c r="P13" s="39"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="68">
+      <c r="B14" s="70">
         <v>4</v>
       </c>
       <c r="C14" s="25">
@@ -1771,7 +1837,7 @@
       <c r="G14" s="31">
         <v>120</v>
       </c>
-      <c r="H14" s="66">
+      <c r="H14" s="72">
         <f>SUM(G14:G20)</f>
         <v>826</v>
       </c>
@@ -1792,7 +1858,7 @@
       <c r="P14" s="36"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="69"/>
+      <c r="B15" s="71"/>
       <c r="C15" s="25">
         <v>43207</v>
       </c>
@@ -1808,7 +1874,7 @@
       <c r="G15" s="31">
         <v>190</v>
       </c>
-      <c r="H15" s="67"/>
+      <c r="H15" s="73"/>
       <c r="J15" s="45">
         <v>13</v>
       </c>
@@ -1826,7 +1892,7 @@
       <c r="P15" s="51"/>
     </row>
     <row r="16" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="69"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="25">
         <v>43208</v>
       </c>
@@ -1842,7 +1908,7 @@
       <c r="G16" s="31">
         <v>30</v>
       </c>
-      <c r="H16" s="67"/>
+      <c r="H16" s="73"/>
       <c r="J16" s="53">
         <v>14</v>
       </c>
@@ -1860,7 +1926,7 @@
       <c r="P16" s="37"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="69"/>
+      <c r="B17" s="71"/>
       <c r="C17" s="25">
         <v>43208</v>
       </c>
@@ -1876,10 +1942,10 @@
       <c r="G17" s="31">
         <v>100</v>
       </c>
-      <c r="H17" s="67"/>
+      <c r="H17" s="73"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="69"/>
+      <c r="B18" s="71"/>
       <c r="C18" s="46">
         <v>43214</v>
       </c>
@@ -1895,10 +1961,10 @@
       <c r="G18" s="50">
         <v>100</v>
       </c>
-      <c r="H18" s="67"/>
+      <c r="H18" s="73"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B19" s="69"/>
+      <c r="B19" s="71"/>
       <c r="C19" s="25">
         <v>43222</v>
       </c>
@@ -1914,10 +1980,10 @@
       <c r="G19" s="31">
         <v>135</v>
       </c>
-      <c r="H19" s="67"/>
+      <c r="H19" s="73"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B20" s="69"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="46">
         <v>43223</v>
       </c>
@@ -1933,10 +1999,10 @@
       <c r="G20" s="50">
         <v>151</v>
       </c>
-      <c r="H20" s="67"/>
+      <c r="H20" s="73"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B21" s="71">
+      <c r="B21" s="69">
         <v>5</v>
       </c>
       <c r="C21" s="25">
@@ -1954,12 +2020,12 @@
       <c r="G21" s="31">
         <v>210</v>
       </c>
-      <c r="H21" s="70">
+      <c r="H21" s="68">
         <v>930</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B22" s="71"/>
+      <c r="B22" s="69"/>
       <c r="C22" s="25">
         <v>43230</v>
       </c>
@@ -1975,10 +2041,10 @@
       <c r="G22" s="31">
         <v>360</v>
       </c>
-      <c r="H22" s="70"/>
+      <c r="H22" s="68"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B23" s="71"/>
+      <c r="B23" s="69"/>
       <c r="C23" s="25">
         <v>43231</v>
       </c>
@@ -1994,32 +2060,53 @@
       <c r="G23" s="31">
         <v>360</v>
       </c>
-      <c r="H23" s="70"/>
-    </row>
-    <row r="24" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="72">
+      <c r="H23" s="68"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="57">
         <v>6</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="46">
         <v>43251</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="F24" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="50">
         <v>360</v>
       </c>
-      <c r="H24" s="73">
+      <c r="H24" s="56">
         <v>360</v>
       </c>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B25" s="76">
+        <v>7</v>
+      </c>
+      <c r="C25" s="25">
+        <v>43278</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="31">
+        <v>180</v>
+      </c>
+      <c r="H25" s="77">
+        <v>300</v>
+      </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -2030,7 +2117,24 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="74"/>
+      <c r="C26" s="32">
+        <v>43278</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="38">
+        <v>120</v>
+      </c>
+      <c r="H26" s="75"/>
       <c r="O26" s="3"/>
       <c r="P26" s="54"/>
       <c r="Q26" s="54"/>
@@ -2130,7 +2234,9 @@
       <c r="W34" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="B25:B26"/>
     <mergeCell ref="H21:H23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B14:B20"/>

</xml_diff>